<commit_message>
updated massSpec sasprogram for merging anotation to analysis datasets and associated documenation
</commit_message>
<xml_diff>
--- a/shaver_metaanalysis_2022/documentation/bff_and_qc_slaw_output.xlsx
+++ b/shaver_metaanalysis_2022/documentation/bff_and_qc_slaw_output.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="144">
   <si>
     <t xml:space="preserve">SLAW on Gtech data</t>
   </si>
@@ -2529,11 +2529,11 @@
   </si>
   <si>
     <t xml:space="preserve">4 metabolomics workbench upload:
-Analysis ready datasets, ranked and unranked with mz and rt uploaded to HPG for brie
+Analysis ready datasets, ranked and unranked with ALL annotations uploaded to HPG for brie
     4 after decimal place for m/z and 2 after for RT</t>
   </si>
   <si>
-    <t xml:space="preserve">massSpec_datasets_4_metabolomicsWorkbench.sas</t>
+    <t xml:space="preserve">massSpec_datasets_4_metabolomicsWorkbench_02amm.sas</t>
   </si>
   <si>
     <r>
@@ -2560,7 +2560,41 @@
 rp_pos_analysisReady_rank_sbys.tsv
 rp_pos_analysisReady_sbys.tsv
 hilic_pos_analysisReady_rank_sbys.tsv
-Hilicp_pos_analysisReady_sbys.tsv</t>
+Hilicp_pos_analysisReady_sbys.tsv
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+McIntyre_Lab/CID/sweet16/SLAW_UGA_Output/text_data/
+Annotation datasets:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+meta_analysis_rp_neg_SLAW_output_0xBFF_PH_annot.tsv
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">meta_analysis_rp_pos_SLAW_output_0xBFF_PH_annot.tsv
+meta_analysis_hilic_pos_SLAW_output_0xBFF_PH_annot.tsv</t>
     </r>
   </si>
   <si>
@@ -2583,16 +2617,267 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">
-rp_neg_analysisReady_sbys_wAnno.tsv
-rp_neg_analysisReady_rank_sbys_wAnno.tsv
-rp_pos_analysisReady_sbys_wAnno.tsv
-rp_pos_analysisReady_rank_sbys_wAnno.tsv
-hilic_pos_analysisReady_sbys_wAnno.tsv
-Hilic_pos_analysisReady_rank_sbys_wAnno.tsv</t>
+rp_neg_analysisReady_sbys_wAnno_full.tsv
+rp_neg_analysisReady_rank_sbys_wAnno</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_full</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.tsv
+rp_pos_analysisReady_sbys_wAnno</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_full</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.tsv
+rp_pos_analysisReady_rank_sbys_wAnno</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_full</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.tsv
+hilic_pos_analysisReady_sbys_wAnno</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_full</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.tsv
+Hilic_pos_analysisReady_rank_sbys_wAnno</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_full</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.tsv</t>
     </r>
   </si>
   <si>
     <t xml:space="preserve">uploaded files for workbench to hpg for brie</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">McIntyre_Lab/CID/sweet16/SLAW_UGA_Output/analysisReady_datasets:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+rp_neg_analysisReady_sbys_wAnno</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_full</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.tsv
+rp_neg_analysisReady_rank_sbys_wAnno</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_full</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.tsv
+rp_pos_analysisReady_sbys_wAnno</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_full</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.tsv
+rp_pos_analysisReady_rank_sbys_wAnno</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_full</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.tsv
+hilic_pos_analysisReady_sbys_wAnno</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_full</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.tsv
+Hilic_pos_analysisReady_rank_sbys_wAnno</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_full</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.tsv</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">scp to:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/blue/mcintyre-cid/share/sweet16/SLAW_UGA_Output_meta/analysisReady_datasets
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">rp_neg_analysisReady_sbys_wAnno_full.tsv
+rp_neg_analysisReady_rank_sbys_wAnno_full.tsv
+rp_pos_analysisReady_sbys_wAnno_full.tsv
+rp_pos_analysisReady_rank_sbys_wAnno_full.tsv
+hilic_pos_analysisReady_sbys_wAnno_full.tsv
+Hilic_pos_analysisReady_rank_sbys_wAnno_full.tsv</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">meta pathway analysis on following 3 strains
@@ -3126,7 +3411,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3193,6 +3478,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -3367,11 +3657,11 @@
   </sheetPr>
   <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G70" activeCellId="0" sqref="G70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="78.5"/>
@@ -3856,7 +4146,7 @@
       </c>
     </row>
     <row r="67" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="68" s="5" customFormat="true" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" s="5" customFormat="true" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="5" t="s">
         <v>98</v>
       </c>
@@ -3871,18 +4161,21 @@
       </c>
     </row>
     <row r="69" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="70" s="5" customFormat="true" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" s="5" customFormat="true" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="5" t="s">
         <v>102</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
+      </c>
+      <c r="G70" s="8" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="71" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="72" s="5" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E72" s="5" t="s">
         <v>78</v>
@@ -3891,60 +4184,60 @@
     <row r="73" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="76" s="5" customFormat="true" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C76" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F76" s="8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="77" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="78" s="5" customFormat="true" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D78" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F78" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="E78" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="F78" s="8" t="s">
-        <v>109</v>
-      </c>
       <c r="G78" s="8" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="79" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="80" s="5" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C80" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G80" s="8" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="81" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3953,16 +4246,16 @@
     <row r="82" s="5" customFormat="true" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="0"/>
       <c r="C82" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F82" s="8" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="83" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3972,19 +4265,19 @@
     <row r="84" s="5" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="0"/>
       <c r="C84" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="85" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4001,16 +4294,16 @@
     <row r="88" s="5" customFormat="true" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0"/>
       <c r="C88" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F88" s="8" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G88" s="8" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="89" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4019,19 +4312,19 @@
     <row r="90" s="5" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="0"/>
       <c r="C90" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F90" s="8" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="91" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4040,19 +4333,19 @@
     <row r="92" s="5" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="0"/>
       <c r="C92" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F92" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated mass spec doc
</commit_message>
<xml_diff>
--- a/shaver_metaanalysis_2022/documentation/bff_and_qc_slaw_output.xlsx
+++ b/shaver_metaanalysis_2022/documentation/bff_and_qc_slaw_output.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="152">
   <si>
     <t xml:space="preserve">SLAW on Gtech data</t>
   </si>
@@ -1428,8 +1428,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">
-BFF_corrected_hilic_neg_with_rt_mz_solv_filt.txt  BFF_corrected_rp_neg_with_rt_mz_solv_filt.txt  
+      <t xml:space="preserve">BFF_corrected_hilic_neg_with_rt_mz_solv_filt.txt  BFF_corrected_rp_neg_with_rt_mz_solv_filt.txt  
 BFF_corrected_hilic_pos_with_rt_mz_solv_filt.txt  BFF_corrected_rp_pos_with_rt_mz_solv_filt.txt
 feature_filtering_README.txt</t>
     </r>
@@ -1456,8 +1455,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">
-BFF_corrected_hilic_neg_with_rt_mz_solv_filt.txt  BFF_corrected_rp_neg_with_rt_mz_solv_filt.txt  
+      <t xml:space="preserve">BFF_corrected_hilic_neg_with_rt_mz_solv_filt.txt  BFF_corrected_rp_neg_with_rt_mz_solv_filt.txt  
 BFF_corrected_hilic_pos_with_rt_mz_solv_filt.txt  BFF_corrected_rp_pos_with_rt_mz_solv_filt.txt
 feature_filtering_README.txt</t>
     </r>
@@ -1602,14 +1600,53 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">
-CV
+      <t xml:space="preserve">CV
 Distributions
 PCA
 SED
-By batch
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">By batch
 By strain_w_poolPD
-*** NOTE that PCA requires design file WITHOUT missing rows in group column!</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">*** NOTE that PCA requires design file WITHOUT missing rows in group column!</t>
     </r>
   </si>
   <si>
@@ -1834,14 +1871,53 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">
-CV
+      <t xml:space="preserve">CV
 Distributions
 PCA
 SED
-By batch
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">By batch
 By strain_w_poolPD
-*** NOTE that PCA requires design file WITHOUT missing rows in group column!</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">*** NOTE that PCA requires design file WITHOUT missing rows in group column!</t>
     </r>
   </si>
   <si>
@@ -2061,14 +2137,53 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">
-CV
+      <t xml:space="preserve">CV
 Distributions
 PCA
 SED
-By batch
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">By batch
 By strain_w_poolPD
-*** NOTE that PCA requires design file WITHOUT missing rows in group column!
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">*** NOTE that PCA requires design file WITHOUT missing rows in group column!
 </t>
     </r>
   </si>
@@ -2306,8 +2421,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">
-BFF_corrected_rp_neg_with_rt_mz_solv_filt.txt  
+      <t xml:space="preserve">BFF_corrected_rp_neg_with_rt_mz_solv_filt.txt  
 BFF_corrected_rp_pos_with_rt_mz_solv_filt.txt
 BFF_corrected_hilic_pos_with_rt_mz_solv_filt.txt  </t>
     </r>
@@ -2412,7 +2526,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">By pathway:
+      <t xml:space="preserve">
+By pathway:
 </t>
     </r>
     <r>
@@ -2445,7 +2560,27 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/McIntyre_Lab/CID/sweet16/SLAW_UGA_Output/comparing_models/&amp;dataout._plot.csv
-Dataout = ${tech}_${path}_4_upset
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Dataout = ${tech}_${path}_4_upset
     e.g. rp_neg_TCA_4_upset
 </t>
     </r>
@@ -2457,7 +2592,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Design:
+      <t xml:space="preserve">
+Design:
 </t>
     </r>
     <r>
@@ -2468,7 +2604,27 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/McIntyre_Lab/CID/sweet16/SLAW_UGA_Output/comparing_models/upset_plot_design_file_&amp;path._sig.csv
-/McIntyre_Lab/CID/sweet16/SLAW_UGA_Output/comparing_models/upset_plot_design_file_&amp;path._ge_pd1074.csv
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/McIntyre_Lab/CID/sweet16/SLAW_UGA_Output/comparing_models/upset_plot_design_file_&amp;path._ge_pd1074.csv
 </t>
     </r>
   </si>
@@ -2554,12 +2710,51 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">
-rp_neg_analysisReady_rank_sbys.tsv
+      <t xml:space="preserve">rp_neg_analysisReady_rank_sbys.tsv
 rp_neg_analysisReady_sbys.tsv
-rp_pos_analysisReady_rank_sbys.tsv
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">rp_pos_analysisReady_rank_sbys.tsv
 rp_pos_analysisReady_sbys.tsv
-hilic_pos_analysisReady_rank_sbys.tsv
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">hilic_pos_analysisReady_rank_sbys.tsv
 Hilicp_pos_analysisReady_sbys.tsv
 </t>
     </r>
@@ -2583,17 +2778,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">
-meta_analysis_rp_neg_SLAW_output_0xBFF_PH_annot.tsv
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">meta_analysis_rp_pos_SLAW_output_0xBFF_PH_annot.tsv
+      <t xml:space="preserve">meta_analysis_rp_neg_SLAW_output_0xBFF_PH_annot.tsv
+meta_analysis_rp_pos_SLAW_output_0xBFF_PH_annot.tsv
 meta_analysis_hilic_pos_SLAW_output_0xBFF_PH_annot.tsv</t>
     </r>
   </si>
@@ -2615,267 +2801,143 @@
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-rp_neg_analysisReady_sbys_wAnno_full.tsv
-rp_neg_analysisReady_rank_sbys_wAnno</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_full</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.tsv
-rp_pos_analysisReady_sbys_wAnno</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_full</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.tsv
-rp_pos_analysisReady_rank_sbys_wAnno</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_full</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.tsv
-hilic_pos_analysisReady_sbys_wAnno</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_full</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.tsv
-Hilic_pos_analysisReady_rank_sbys_wAnno</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_full</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.tsv</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">uploaded files for workbench to hpg for brie</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">McIntyre_Lab/CID/sweet16/SLAW_UGA_Output/analysisReady_datasets:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-rp_neg_analysisReady_sbys_wAnno</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_full</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.tsv
-rp_neg_analysisReady_rank_sbys_wAnno</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_full</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.tsv
-rp_pos_analysisReady_sbys_wAnno</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_full</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.tsv
-rp_pos_analysisReady_rank_sbys_wAnno</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_full</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.tsv
-hilic_pos_analysisReady_sbys_wAnno</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_full</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.tsv
-Hilic_pos_analysisReady_rank_sbys_wAnno</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_full</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.tsv</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">scp to:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/blue/mcintyre-cid/share/sweet16/SLAW_UGA_Output_meta/analysisReady_datasets
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
       </rPr>
       <t xml:space="preserve">rp_neg_analysisReady_sbys_wAnno_full.tsv
 rp_neg_analysisReady_rank_sbys_wAnno_full.tsv
-rp_pos_analysisReady_sbys_wAnno_full.tsv
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">rp_pos_analysisReady_sbys_wAnno_full.tsv
 rp_pos_analysisReady_rank_sbys_wAnno_full.tsv
-hilic_pos_analysisReady_sbys_wAnno_full.tsv
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">hilic_pos_analysisReady_sbys_wAnno_full.tsv
+Hilic_pos_analysisReady_rank_sbys_wAnno_full.tsv</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">uploaded files for workbench to hpg for brie</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">scp to:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/blue/mcintyre-cid/share/sweet16/SLAW_UGA_Output_meta/analysisReady_datasets
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">rp_neg_analysisReady_sbys_wAnno_full.tsv
+rp_neg_analysisReady_rank_sbys_wAnno_full.tsv
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">rp_pos_analysisReady_sbys_wAnno_full.tsv
+rp_pos_analysisReady_rank_sbys_wAnno_full.tsv
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">hilic_pos_analysisReady_sbys_wAnno_full.tsv
 Hilic_pos_analysisReady_rank_sbys_wAnno_full.tsv</t>
     </r>
   </si>
@@ -2933,7 +2995,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Nmr effect sizes (cdcl3, d2o):
+      <t xml:space="preserve">
+Nmr effect sizes (cdcl3, d2o):
 </t>
     </r>
     <r>
@@ -2977,7 +3040,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Metabolites across top:
+      <t xml:space="preserve">
+Metabolites across top:
 </t>
     </r>
     <r>
@@ -2991,6 +3055,17 @@
 SHARE/McIntyre_Lab/CID/sweet16/analysis_massSpec_and_NMR/effectSizes_flipped_MassSpec_NMR.tsv
 </t>
     </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Run MMC
@@ -3032,7 +3107,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Effect sizes across top:
+      <t xml:space="preserve">
+Effect sizes across top:
 </t>
     </r>
     <r>
@@ -3054,7 +3130,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Metabolites across top:
+      <t xml:space="preserve">
+Metabolites across top:
 </t>
     </r>
     <r>
@@ -3105,10 +3182,29 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">
-MA_FE_rank_byPath_${VAR}_${PATHWAY}_report.tsv 
+      <t xml:space="preserve">MA_FE_rank_byPath_${VAR}_${PATHWAY}_report.tsv 
 MA_FE_rank_byPath_${VAR}_${PATHWAY}_SMD_summary.tsv
-VAR=rp_neg, rp_pos or hilic_pos
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">VAR=rp_neg, rp_pos or hilic_pos
 PATHWAY=NI_no_N2</t>
     </r>
   </si>
@@ -3250,7 +3346,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Output for upset plot:
+      <t xml:space="preserve">
+Output for upset plot:
 </t>
     </r>
     <r>
@@ -3271,7 +3368,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Design for heatmap:
+      <t xml:space="preserve">
+Design for heatmap:
 </t>
     </r>
     <r>
@@ -3292,7 +3390,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Design needed for upset plot
+      <t xml:space="preserve">
+Design needed for upset plot
 </t>
     </r>
     <r>
@@ -3339,6 +3438,17 @@
       <t xml:space="preserve">McIntyre_Lab/CID/sweet16/SLAW_UGA_Output/meta_analysis_&amp;tech./MA_byStrain_sig_4_heatmap.tsv
 </t>
     </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">PROJ/SLAW_UGA_Output/meta_analysis_${TYPE}/MMC_heatmap_MA_byStrain_sig_${TYPE}.pdf
@@ -3355,7 +3465,7 @@
     <t xml:space="preserve"> $SCRIPTS/upset_plot.py</t>
   </si>
   <si>
-    <t xml:space="preserve">run_upset_plot_byStrain.sh</t>
+    <t xml:space="preserve">McIntyre_Lab/CID/sweet16/scripts/massSpec/meta_analysis/run_upset_plot_byStrain.sh</t>
   </si>
   <si>
     <r>
@@ -3387,7 +3497,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Design needed for upset plot
+      <t xml:space="preserve">
+Design needed for upset plot
 </t>
     </r>
     <r>
@@ -3402,6 +3513,316 @@
   </si>
   <si>
     <t xml:space="preserve">$PROJ/SLAW_UGA_Output/meta_analysis_${i}/upsetPlot_byStrain_sig_${i}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rsync SIRIUS output from Brie and Amanda from hpg to mclab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">McIntyre_Lab/CID/sweet16/scripts
+rsync_sweet16_MA_sirius_output_hpg_2_mclab.sh</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">create supplementary files:  PH, flag_sig_X, all annotations, Sirius output 
+Import needed files:
+  effect sizes and pvalues by strain
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  effect sizes and pvalues by pathway
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+  PH from analysis ready datasets
+  Annotations (ms slaw) 
+  Mol structure (ms sirius)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">import_2_create_suppl_datasets.sas
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">mass spec input files:
+Effect sizes and pvalues by strain: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> /McIntyre_Lab/CID/sweet16/SLAW_UGA_Output/meta_analysis_&amp;tech./MA_FE_rank_byMut_&amp;tech._&amp;strain._SMD_summary.tsv
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Effect sizes and pvalues by pathway: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">McIntyre_Lab/CID/sweet16/SLAW_UGA_Output/meta_analysis_&amp;tech./MA_FE_rank_byPath_&amp;tech._&amp;path._SMD_summary.tsv"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PH analysis ready data:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">McIntyre_Lab/CID/sweet16/SLAW_UGA_Output/analysisReady_datasets/&amp;datain.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Slaw output annotation file
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">McIntyre_Lab/CID/sweet16/SLAW_UGA_Output/text_data/meta_analysis_&amp;tech._SLAW_output_0xBFF_PH_annot.tsv
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+Sirius output – molecular structure info
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">McIntyre_Lab/CID/sweet16/MA_SIRIUS_output/SIRIUS_output_mergedIDs/SIRIUS_MA_&amp;tech._mergedID.csv
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">nmr input files:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Effect sizes and pvalues by strain: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">McIntyre_Lab/CID/sweet16/nmr/meta_analysis/MA_fixedEffect_NMR_&amp;tech._rank_&amp;strain._&amp;tech._SMD_summary.tsv
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Effect sizes and pvalues by pathway: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">McIntyre_Lab/CID/sweet16/nmr/meta_analysis/MA_fixedEffect_pathway_NMR_&amp;tech._rank_&amp;path._summary.tsv
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">PH analysis ready data:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">McIntyre_Lab/CID/sweet16/nmr/ready_&amp;tech._PH_sbys.tsv
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">sas work datasets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create supplementary files:  PH, flag_sig_X, all annotations, Sirius output   
+Merge above files
+rename TCA = CM
+rename NI = NS
+    mass spec:
+        for each tech: (1) merge MA results (strain and path), all annotations and sirius output
+                             (2) PH analysis ready
+                             (3) export design files with pair info
+        inputs: work.ma_&amp;tech._&amp;strain 
+                  work.ma_&amp;tech._&amp;path
+                  work.ph_&amp;tech.
+                  work.sr_&amp;tech. 
+                  dsgn_GT_RP_NEG_pairs_slaw.tsv
+                  dsgn_GT_RP_POS_pairs_slaw.tsv
+                  dsgn_GT_HILIC_POS_pairs_slaw.tsv
+  nmr
+        for each tech: (1) merge MA results (strain and path)
+                             (2) ppm analysis ready
+                             (3) export design files with pair info
+        inputs: work.ma_&amp;tech._&amp;strain.
+                  work.ma_&amp;tech._&amp;path.
+                  work.ph_&amp;tech.
+                  nmr/dsgn_cdcl3_sbys.tsv
+                  Nmr/dsgn_d2o_sbys.tsv
+All outputs in:  McIntyre_Lab/CID/sweet16/manuscript/supplemental_data
+Create list of meta table columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">merge_2_create_suppl_datasets.sas</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">manu.suppl_&amp;tech._meta_table
+McIntyre_Lab/CID/sweet16/manuscript/supplemental_data/suppl_&amp;tech._meta_table.tsv"
+manu.suppl_&amp;tech._&amp;type._table
+McIntyre_Lab/CID/sweet16/manuscript/supplemental_data/suppl_&amp;tech._&amp;type._table.tsv
+export design files -- mass spec (all techs are ID!)
+manu.design_mass_spec 
+McIntyre_Lab/CID/sweet16/manuscript/supplemental_data/design_mass_spec.tsv
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">export design files – nmr, cdcl3 and d20 are different!
+manu.design_nmr_&amp;tech.
+McIntyre_Lab/CID/sweet16/manuscript/supplemental_data/design_nmr_&amp;tech..tsv
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+List of column headers for meta table:
+manu.meta_table_columns
+McIntyre_Lab/CID/sweet16/manuscript/supplemental_data/meta_table_columns.tsv</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3411,7 +3832,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3484,6 +3905,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -3533,7 +3960,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3576,6 +4003,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -3655,19 +4086,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H92"/>
+  <dimension ref="A1:H98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G70" activeCellId="0" sqref="G70"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C79" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C82" activeCellId="0" sqref="C82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="78.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="41.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="57.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="70.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="73.22"/>
   </cols>
   <sheetData>
@@ -3949,7 +4380,7 @@
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" s="5" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" s="5" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="3" t="s">
         <v>56</v>
       </c>
@@ -4095,7 +4526,7 @@
       </c>
     </row>
     <row r="61" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="62" s="5" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" s="5" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="5" t="s">
         <v>86</v>
       </c>
@@ -4113,7 +4544,7 @@
       </c>
     </row>
     <row r="63" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="64" s="5" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" s="5" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="5" t="s">
         <v>91</v>
       </c>
@@ -4166,16 +4597,16 @@
         <v>102</v>
       </c>
       <c r="F70" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G70" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="G70" s="8" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="71" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="72" s="5" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E72" s="5" t="s">
         <v>78</v>
@@ -4184,60 +4615,60 @@
     <row r="73" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D74" s="0" t="s">
         <v>106</v>
-      </c>
-      <c r="D74" s="0" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="76" s="5" customFormat="true" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C76" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D76" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="E76" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="E76" s="8" t="s">
+      <c r="F76" s="8" t="s">
         <v>110</v>
-      </c>
-      <c r="F76" s="8" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="77" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="78" s="5" customFormat="true" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D78" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="E78" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E78" s="5" t="s">
+      <c r="F78" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="G78" s="8" t="s">
         <v>114</v>
-      </c>
-      <c r="F78" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="G78" s="8" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="79" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="80" s="5" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C80" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D80" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D80" s="5" t="s">
+      <c r="E80" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E80" s="5" t="s">
+      <c r="F80" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="F80" s="5" t="s">
+      <c r="G80" s="8" t="s">
         <v>119</v>
-      </c>
-      <c r="G80" s="8" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="81" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4246,16 +4677,16 @@
     <row r="82" s="5" customFormat="true" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="0"/>
       <c r="C82" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D82" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="F82" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="F82" s="8" t="s">
+      <c r="G82" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="G82" s="5" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="83" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4265,19 +4696,19 @@
     <row r="84" s="5" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="0"/>
       <c r="C84" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D84" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="E84" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="E84" s="5" t="s">
+      <c r="F84" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="F84" s="5" t="s">
+      <c r="G84" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="G84" s="5" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="85" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4294,16 +4725,16 @@
     <row r="88" s="5" customFormat="true" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0"/>
       <c r="C88" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D88" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="F88" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="F88" s="8" t="s">
+      <c r="G88" s="8" t="s">
         <v>132</v>
-      </c>
-      <c r="G88" s="8" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="89" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4312,19 +4743,19 @@
     <row r="90" s="5" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="0"/>
       <c r="C90" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D90" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="D90" s="5" t="s">
+      <c r="E90" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="E90" s="5" t="s">
+      <c r="F90" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="F90" s="8" t="s">
+      <c r="G90" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="G90" s="5" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="91" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4333,19 +4764,57 @@
     <row r="92" s="5" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="0"/>
       <c r="C92" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D92" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D92" s="5" t="s">
+      <c r="E92" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="E92" s="5" t="s">
+      <c r="F92" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="F92" s="8" t="s">
+      <c r="G92" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="G92" s="5" t="s">
+    </row>
+    <row r="94" s="5" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C94" s="5" t="s">
         <v>143</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="95" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="96" s="5" customFormat="true" ht="370.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C96" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F96" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="G96" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="97" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="98" s="5" customFormat="true" ht="359.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C98" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D98" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="G98" s="5" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>